<commit_message>
Added validators for inputs
</commit_message>
<xml_diff>
--- a/Current Patients/12345/DataBases/Data/12345_Anthropometrics_Source.xlsx
+++ b/Current Patients/12345/DataBases/Data/12345_Anthropometrics_Source.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,17 +641,79 @@
       <c r="P3" t="n">
         <v>234</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr">
         <is>
           <t>234</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
           <t>234</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>222</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>07/17/2020</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>22</v>
+      </c>
+      <c r="H4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I4" t="n">
+        <v>444</v>
+      </c>
+      <c r="J4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K4" t="n">
+        <v>33</v>
+      </c>
+      <c r="L4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M4" t="n">
+        <v>33</v>
+      </c>
+      <c r="N4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O4" t="n">
+        <v>44</v>
+      </c>
+      <c r="P4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>sdfsf</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>sdfsfsdfsfsfs</t>
         </is>
       </c>
     </row>

</xml_diff>